<commit_message>
MEC identifiers version 2311
Update Monthly Enterprise Channel identifiers for version 2311 (Build 17029.20140
</commit_message>
<xml_diff>
--- a/Microsoft 365/Monthly Enterprise Channel/outlookmmseditcontrols.xlsx
+++ b/Microsoft 365/Monthly Enterprise Channel/outlookmmseditcontrols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27315"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcoard\OneDrive - Microsoft\Documents\RibbonX Upload\MEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TcidDocs\MECOct2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{073235D1-4881-47F5-A5DC-BEEE8F8C5DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81CF2CF4-F8A8-406E-B062-70288F8B61D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="43200" windowHeight="23325"/>
+    <workbookView xWindow="0" yWindow="5415" windowWidth="51600" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="outlookmmseditcontrols" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="146">
   <si>
     <t>Policy ID</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>OutlookFeedbackUIF</t>
+  </si>
+  <si>
+    <t>OfficeFeedbackBackstage</t>
   </si>
   <si>
     <t>Column1</t>
@@ -461,25 +464,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -487,7 +490,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -495,7 +498,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -503,35 +506,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -539,7 +542,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -547,14 +550,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -562,14 +565,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -577,7 +580,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -585,14 +588,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -646,19 +649,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -669,19 +672,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -692,19 +695,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -715,19 +718,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -738,19 +741,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -761,19 +764,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -809,7 +812,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -999,8 +1002,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I152" totalsRowShown="0">
-  <autoFilter ref="A1:I152"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I153" totalsRowShown="0">
+  <autoFilter ref="A1:I153"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Control Name"/>
     <tableColumn id="2" name="Control Type"/>
@@ -1027,39 +1030,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1111,7 +1114,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1222,13 +1225,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1237,6 +1233,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1301,11 +1304,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1313,26 +1336,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="1" max="1" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.625" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1358,10 +1381,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +1418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1412,7 +1435,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1452,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1469,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1463,7 +1486,7 @@
         <v>25419</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1480,7 +1503,7 @@
         <v>16164</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1517,7 @@
         <v>13289</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1511,7 +1534,7 @@
         <v>12597</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1531,7 +1554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1551,7 +1574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1571,7 +1594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1591,7 +1614,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1608,7 +1631,7 @@
         <v>13343</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1628,7 +1651,7 @@
         <v>13312</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1648,7 +1671,7 @@
         <v>13315</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1691,7 @@
         <v>13313</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1691,7 +1714,7 @@
         <v>13318</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1711,7 +1734,7 @@
         <v>13318</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1728,7 +1751,7 @@
         <v>14349</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1748,7 +1771,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1768,7 +1791,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1785,7 +1808,7 @@
         <v>13293</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1805,7 +1828,7 @@
         <v>13316</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1828,7 +1851,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1851,7 +1874,7 @@
         <v>20868</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1871,7 +1894,7 @@
         <v>13303</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +1914,7 @@
         <v>13317</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1914,7 +1937,7 @@
         <v>13319</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1937,7 +1960,7 @@
         <v>2707</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1954,7 +1977,7 @@
         <v>13294</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1974,7 +1997,7 @@
         <v>13308</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1994,7 +2017,7 @@
         <v>13309</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2008,7 +2031,7 @@
         <v>22110</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2025,7 +2048,7 @@
         <v>22111</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2045,7 +2068,7 @@
         <v>19623</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2065,7 +2088,7 @@
         <v>19624</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2085,7 +2108,7 @@
         <v>19625</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2102,7 +2125,7 @@
         <v>22112</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2122,7 +2145,7 @@
         <v>22113</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2142,7 +2165,7 @@
         <v>22338</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2159,7 +2182,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -2176,7 +2199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2193,7 +2216,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2210,7 +2233,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2227,7 +2250,7 @@
         <v>11323</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2244,7 +2267,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2261,7 +2284,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2278,7 +2301,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2295,7 +2318,7 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2312,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -2329,7 +2352,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="B54" t="s">
         <v>9</v>
       </c>
@@ -2343,7 +2366,7 @@
         <v>19211</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="B55" t="s">
         <v>9</v>
       </c>
@@ -2357,7 +2380,7 @@
         <v>19212</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="B56" t="s">
         <v>9</v>
       </c>
@@ -2371,7 +2394,7 @@
         <v>19214</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="B57" t="s">
         <v>9</v>
       </c>
@@ -2385,7 +2408,7 @@
         <v>19213</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="B58" t="s">
         <v>9</v>
       </c>
@@ -2399,7 +2422,7 @@
         <v>19215</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -2416,7 +2439,7 @@
         <v>9340</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2433,7 +2456,7 @@
         <v>5933</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2450,7 +2473,7 @@
         <v>7714</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2467,7 +2490,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -2484,7 +2507,7 @@
         <v>16164</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -2501,7 +2524,7 @@
         <v>32712</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2518,7 +2541,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -2535,7 +2558,7 @@
         <v>24438</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -2552,7 +2575,7 @@
         <v>22143</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2569,7 +2592,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2586,7 +2609,7 @@
         <v>7391</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2603,7 +2626,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2620,7 +2643,7 @@
         <v>25419</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2637,7 +2660,7 @@
         <v>22377</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2654,7 +2677,7 @@
         <v>5598</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2671,7 +2694,7 @@
         <v>20108</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2688,7 +2711,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2705,7 +2728,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2722,7 +2745,7 @@
         <v>26904</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2739,7 +2762,7 @@
         <v>27010</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2756,7 +2779,7 @@
         <v>27007</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2773,7 +2796,7 @@
         <v>27006</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2790,7 +2813,7 @@
         <v>27085</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2807,7 +2830,7 @@
         <v>27142</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2824,7 +2847,7 @@
         <v>27805</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2841,7 +2864,7 @@
         <v>27877</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2858,7 +2881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -2875,7 +2898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2892,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2909,7 +2932,7 @@
         <v>27964</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2926,7 +2949,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="B90" t="s">
         <v>9</v>
       </c>
@@ -2937,7 +2960,7 @@
         <v>33991</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2951,7 +2974,7 @@
         <v>18148</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2968,7 +2991,7 @@
         <v>25295</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2985,7 +3008,7 @@
         <v>34474</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="B94" t="s">
         <v>24</v>
       </c>
@@ -2999,7 +3022,7 @@
         <v>33917</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -3016,7 +3039,7 @@
         <v>33912</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -3033,7 +3056,7 @@
         <v>20423</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -3050,7 +3073,7 @@
         <v>20424</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -3067,7 +3090,7 @@
         <v>20425</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -3084,7 +3107,7 @@
         <v>20426</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -3101,7 +3124,7 @@
         <v>20440</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -3118,7 +3141,7 @@
         <v>20441</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -3135,7 +3158,7 @@
         <v>32646</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -3152,7 +3175,7 @@
         <v>20442</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -3169,7 +3192,7 @@
         <v>20443</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -3186,7 +3209,7 @@
         <v>20444</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -3203,7 +3226,7 @@
         <v>20445</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -3220,7 +3243,7 @@
         <v>18792</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8">
       <c r="B108" t="s">
         <v>9</v>
       </c>
@@ -3231,7 +3254,7 @@
         <v>33940</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8">
       <c r="B109" t="s">
         <v>9</v>
       </c>
@@ -3242,7 +3265,7 @@
         <v>33939</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -3256,7 +3279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>61</v>
       </c>
@@ -3270,7 +3293,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>62</v>
       </c>
@@ -3284,7 +3307,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -3298,7 +3321,7 @@
         <v>18244</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -3315,7 +3338,7 @@
         <v>19139</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -3332,7 +3355,7 @@
         <v>19140</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -3346,7 +3369,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3357,7 +3380,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -3371,7 +3394,7 @@
         <v>20802</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3388,7 +3411,7 @@
         <v>24423</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -3405,7 +3428,7 @@
         <v>33755</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -3425,7 +3448,7 @@
         <v>33756</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -3442,7 +3465,7 @@
         <v>24850</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -3459,7 +3482,7 @@
         <v>25368</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3476,7 +3499,7 @@
         <v>24207</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -3493,7 +3516,7 @@
         <v>24952</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -3510,7 +3533,7 @@
         <v>24424</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="B127" t="s">
         <v>9</v>
       </c>
@@ -3527,7 +3550,7 @@
         <v>24421</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -3544,7 +3567,7 @@
         <v>22547</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>125</v>
       </c>
@@ -3561,7 +3584,7 @@
         <v>20511</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -3578,7 +3601,7 @@
         <v>34138</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>127</v>
       </c>
@@ -3598,7 +3621,7 @@
         <v>34139</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -3615,7 +3638,7 @@
         <v>27331</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -3635,7 +3658,7 @@
         <v>27363</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -3655,7 +3678,7 @@
         <v>27364</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -3675,7 +3698,7 @@
         <v>27365</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>132</v>
       </c>
@@ -3695,7 +3718,7 @@
         <v>27366</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>133</v>
       </c>
@@ -3712,7 +3735,7 @@
         <v>18158</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>134</v>
       </c>
@@ -3729,7 +3752,7 @@
         <v>26945</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>135</v>
       </c>
@@ -3743,7 +3766,7 @@
         <v>27265</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>136</v>
       </c>
@@ -3760,7 +3783,7 @@
         <v>27266</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>137</v>
       </c>
@@ -3777,7 +3800,7 @@
         <v>27267</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>138</v>
       </c>
@@ -3794,7 +3817,7 @@
         <v>27545</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -3811,7 +3834,7 @@
         <v>33737</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="B144" t="s">
         <v>9</v>
       </c>
@@ -3828,7 +3851,7 @@
         <v>33739</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -3845,7 +3868,7 @@
         <v>33738</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="B146" t="s">
         <v>9</v>
       </c>
@@ -3862,7 +3885,7 @@
         <v>33740</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>141</v>
       </c>
@@ -3879,7 +3902,7 @@
         <v>27005</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>85</v>
       </c>
@@ -3899,7 +3922,7 @@
         <v>27007</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>142</v>
       </c>
@@ -3916,7 +3939,7 @@
         <v>27021</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>86</v>
       </c>
@@ -3936,7 +3959,7 @@
         <v>27006</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>143</v>
       </c>
@@ -3950,17 +3973,31 @@
         <v>27058</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
+        <v>144</v>
+      </c>
+      <c r="B152" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152" t="s">
+        <v>93</v>
+      </c>
+      <c r="H152">
+        <v>27302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" t="s">
         <v>60</v>
       </c>
-      <c r="B152" t="s">
-        <v>9</v>
-      </c>
-      <c r="C152" t="s">
-        <v>93</v>
-      </c>
-      <c r="H152">
+      <c r="B153" t="s">
+        <v>9</v>
+      </c>
+      <c r="C153" t="s">
+        <v>93</v>
+      </c>
+      <c r="H153">
         <v>11323</v>
       </c>
     </row>

</xml_diff>